<commit_message>
Update: Đánh giá tour, tài liệu
</commit_message>
<xml_diff>
--- a/Document/8.1.ProjectTestCaseSprint1.xlsx
+++ b/Document/8.1.ProjectTestCaseSprint1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN_Document\Document_DaSua\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F3635-22C2-49A5-AED8-95BEAA91F98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFA3302-FFFC-4E79-ACC9-4449412ED378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="896" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1918,7 +1918,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="38" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2387,18 +2387,42 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2414,36 +2438,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2462,17 +2459,26 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2484,22 +2490,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2508,14 +2514,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2550,24 +2556,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2589,17 +2598,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3364,24 +3367,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="112" customFormat="1" ht="24.6">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
-      <c r="E1" s="189"/>
-      <c r="F1" s="189"/>
-      <c r="G1" s="189"/>
-      <c r="H1" s="189"/>
-      <c r="I1" s="189"/>
-      <c r="J1" s="189"/>
-      <c r="K1" s="189"/>
-      <c r="L1" s="189"/>
-      <c r="M1" s="189"/>
-      <c r="N1" s="189"/>
-      <c r="O1" s="189"/>
-      <c r="P1" s="189"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
     </row>
     <row r="2" spans="1:16" s="112" customFormat="1" ht="13.2">
       <c r="A2" s="115"/>
@@ -3405,22 +3408,22 @@
       <c r="A3" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="190" t="s">
+      <c r="B3" s="181" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="190"/>
+      <c r="C3" s="181"/>
       <c r="D3" s="118"/>
-      <c r="E3" s="183" t="s">
+      <c r="E3" s="182" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="191" t="s">
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="183" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="193"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="185"/>
       <c r="L3" s="157"/>
       <c r="M3" s="157"/>
       <c r="N3" s="157"/>
@@ -3429,20 +3432,20 @@
     </row>
     <row r="4" spans="1:16" s="112" customFormat="1" ht="16.8">
       <c r="A4" s="117"/>
-      <c r="B4" s="182"/>
-      <c r="C4" s="182"/>
+      <c r="B4" s="186"/>
+      <c r="C4" s="186"/>
       <c r="D4" s="119"/>
-      <c r="E4" s="183" t="s">
+      <c r="E4" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="183"/>
-      <c r="G4" s="183"/>
-      <c r="H4" s="194" t="s">
+      <c r="F4" s="182"/>
+      <c r="G4" s="182"/>
+      <c r="H4" s="187" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="195"/>
-      <c r="J4" s="195"/>
-      <c r="K4" s="196"/>
+      <c r="I4" s="188"/>
+      <c r="J4" s="188"/>
+      <c r="K4" s="189"/>
       <c r="L4" s="119"/>
       <c r="M4" s="157"/>
       <c r="N4" s="157"/>
@@ -3451,20 +3454,20 @@
     </row>
     <row r="5" spans="1:16" s="112" customFormat="1" ht="16.8">
       <c r="A5" s="117"/>
-      <c r="B5" s="182"/>
-      <c r="C5" s="182"/>
+      <c r="B5" s="186"/>
+      <c r="C5" s="186"/>
       <c r="D5" s="119"/>
-      <c r="E5" s="183" t="s">
+      <c r="E5" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183"/>
-      <c r="H5" s="184">
+      <c r="F5" s="182"/>
+      <c r="G5" s="182"/>
+      <c r="H5" s="192">
         <v>44114</v>
       </c>
-      <c r="I5" s="185"/>
-      <c r="J5" s="185"/>
-      <c r="K5" s="186"/>
+      <c r="I5" s="193"/>
+      <c r="J5" s="193"/>
+      <c r="K5" s="194"/>
       <c r="L5" s="119"/>
       <c r="M5" s="157"/>
       <c r="N5" s="157"/>
@@ -3475,18 +3478,18 @@
       <c r="A6" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="187" t="s">
+      <c r="B6" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
-      <c r="K6" s="187"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="195"/>
+      <c r="H6" s="195"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="195"/>
+      <c r="K6" s="195"/>
       <c r="L6" s="121"/>
       <c r="M6" s="158"/>
       <c r="N6" s="158"/>
@@ -3496,52 +3499,52 @@
     <row r="7" spans="1:16" s="112" customFormat="1" ht="20.25" customHeight="1">
       <c r="A7" s="122"/>
       <c r="B7" s="123"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="196" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188" t="s">
+      <c r="D7" s="196"/>
+      <c r="E7" s="196" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188" t="s">
+      <c r="F7" s="196"/>
+      <c r="G7" s="196" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="188"/>
-      <c r="I7" s="188" t="s">
+      <c r="H7" s="196"/>
+      <c r="I7" s="196" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="188"/>
-      <c r="K7" s="188" t="s">
+      <c r="J7" s="196"/>
+      <c r="K7" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="188"/>
-      <c r="M7" s="180" t="s">
+      <c r="L7" s="196"/>
+      <c r="M7" s="190" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="180"/>
-      <c r="O7" s="181" t="s">
+      <c r="N7" s="190"/>
+      <c r="O7" s="191" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="181"/>
+      <c r="P7" s="191"/>
     </row>
     <row r="8" spans="1:16" s="112" customFormat="1" ht="16.8">
       <c r="A8" s="124"/>
       <c r="B8" s="125"/>
-      <c r="C8" s="188"/>
-      <c r="D8" s="188"/>
-      <c r="E8" s="188"/>
-      <c r="F8" s="188"/>
-      <c r="G8" s="188"/>
-      <c r="H8" s="188"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="188"/>
-      <c r="K8" s="188"/>
-      <c r="L8" s="188"/>
-      <c r="M8" s="180"/>
-      <c r="N8" s="180"/>
-      <c r="O8" s="181"/>
-      <c r="P8" s="181"/>
+      <c r="C8" s="196"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="196"/>
+      <c r="G8" s="196"/>
+      <c r="H8" s="196"/>
+      <c r="I8" s="196"/>
+      <c r="J8" s="196"/>
+      <c r="K8" s="196"/>
+      <c r="L8" s="196"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="191"/>
+      <c r="P8" s="191"/>
     </row>
     <row r="9" spans="1:16" s="113" customFormat="1" ht="22.5" customHeight="1">
       <c r="A9" s="126" t="s">
@@ -4262,13 +4265,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:K4"/>
     <mergeCell ref="M7:N8"/>
     <mergeCell ref="O7:P8"/>
     <mergeCell ref="B5:C5"/>
@@ -4280,6 +4276,13 @@
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="I7:J8"/>
     <mergeCell ref="K7:L8"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4291,7 +4294,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" customHeight="1"/>
@@ -4300,22 +4303,23 @@
     <col min="2" max="2" width="41.5546875" style="168" customWidth="1"/>
     <col min="3" max="3" width="41" style="168" customWidth="1"/>
     <col min="4" max="4" width="41.88671875" style="168" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="168"/>
+    <col min="5" max="5" width="13.21875" style="168" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="168"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="198" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="201"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="200"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A2" s="202"/>
-      <c r="B2" s="203"/>
-      <c r="C2" s="203"/>
-      <c r="D2" s="204"/>
+      <c r="A2" s="201"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="203"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1">
       <c r="A3" s="169" t="s">
@@ -4324,15 +4328,15 @@
       <c r="B3" s="197" t="s">
         <v>302</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="198"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
-      <c r="J3" s="198"/>
-      <c r="K3" s="198"/>
+      <c r="C3" s="254"/>
+      <c r="D3" s="254"/>
+      <c r="E3" s="254"/>
+      <c r="F3" s="253"/>
+      <c r="G3" s="253"/>
+      <c r="H3" s="253"/>
+      <c r="I3" s="253"/>
+      <c r="J3" s="253"/>
+      <c r="K3" s="253"/>
     </row>
     <row r="4" spans="1:11" ht="16.5" customHeight="1">
       <c r="A4" s="170" t="s">
@@ -4478,8 +4482,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:K3"/>
     <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4516,13 +4520,13 @@
       <c r="A1" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="207" t="s">
+      <c r="B1" s="204" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
       <c r="G1" s="80"/>
       <c r="H1" s="81"/>
       <c r="J1" s="80"/>
@@ -4531,13 +4535,13 @@
       <c r="A2" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="208" t="s">
+      <c r="B2" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
       <c r="G2" s="80"/>
       <c r="H2" s="81"/>
       <c r="J2" s="80"/>
@@ -4701,21 +4705,21 @@
       <c r="M9" s="206"/>
     </row>
     <row r="10" spans="1:13" s="77" customFormat="1">
-      <c r="A10" s="205" t="s">
+      <c r="A10" s="207" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="205"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="205"/>
-      <c r="E10" s="205"/>
-      <c r="F10" s="205"/>
-      <c r="G10" s="205"/>
-      <c r="H10" s="205"/>
-      <c r="I10" s="205"/>
-      <c r="J10" s="205"/>
-      <c r="K10" s="205"/>
-      <c r="L10" s="205"/>
-      <c r="M10" s="205"/>
+      <c r="B10" s="207"/>
+      <c r="C10" s="207"/>
+      <c r="D10" s="207"/>
+      <c r="E10" s="207"/>
+      <c r="F10" s="207"/>
+      <c r="G10" s="207"/>
+      <c r="H10" s="207"/>
+      <c r="I10" s="207"/>
+      <c r="J10" s="207"/>
+      <c r="K10" s="207"/>
+      <c r="L10" s="207"/>
+      <c r="M10" s="207"/>
     </row>
     <row r="11" spans="1:13" s="77" customFormat="1" ht="33.6">
       <c r="A11" s="92" t="s">
@@ -5185,12 +5189,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
     <mergeCell ref="A10:M10"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
@@ -5199,6 +5197,12 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="M7:M9"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G11:G15 G17:G25 J11:J16 J18:J26" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -5215,7 +5219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
@@ -5241,13 +5245,13 @@
       <c r="A1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="208" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
       <c r="G1" s="60"/>
       <c r="H1" s="61"/>
       <c r="J1" s="60"/>
@@ -5256,13 +5260,13 @@
       <c r="A2" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="209" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
       <c r="G2" s="60"/>
       <c r="H2" s="61"/>
       <c r="J2" s="60"/>
@@ -5350,64 +5354,64 @@
       <c r="J6" s="65"/>
     </row>
     <row r="7" spans="1:13" s="58" customFormat="1" ht="18">
-      <c r="A7" s="212" t="s">
+      <c r="A7" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="212" t="s">
+      <c r="C7" s="210" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="212" t="s">
+      <c r="D7" s="210" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="213" t="s">
+      <c r="E7" s="214" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="212" t="s">
+      <c r="F7" s="210" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="212" t="s">
+      <c r="G7" s="210" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="212"/>
-      <c r="I7" s="212"/>
-      <c r="J7" s="212" t="s">
+      <c r="H7" s="210"/>
+      <c r="I7" s="210"/>
+      <c r="J7" s="210" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="212"/>
-      <c r="L7" s="212"/>
-      <c r="M7" s="212" t="s">
+      <c r="K7" s="210"/>
+      <c r="L7" s="210"/>
+      <c r="M7" s="210" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="58" customFormat="1" ht="18">
-      <c r="A8" s="212"/>
-      <c r="B8" s="212"/>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="213"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="212" t="s">
+      <c r="A8" s="210"/>
+      <c r="B8" s="210"/>
+      <c r="C8" s="210"/>
+      <c r="D8" s="210"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="210"/>
+      <c r="G8" s="210" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="212"/>
-      <c r="I8" s="212"/>
-      <c r="J8" s="212" t="s">
+      <c r="H8" s="210"/>
+      <c r="I8" s="210"/>
+      <c r="J8" s="210" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="212"/>
-      <c r="L8" s="212"/>
-      <c r="M8" s="212"/>
+      <c r="K8" s="210"/>
+      <c r="L8" s="210"/>
+      <c r="M8" s="210"/>
     </row>
     <row r="9" spans="1:13" s="58" customFormat="1" ht="18">
-      <c r="A9" s="212"/>
-      <c r="B9" s="212"/>
-      <c r="C9" s="212"/>
-      <c r="D9" s="212"/>
-      <c r="E9" s="213"/>
-      <c r="F9" s="212"/>
+      <c r="A9" s="210"/>
+      <c r="B9" s="210"/>
+      <c r="C9" s="210"/>
+      <c r="D9" s="210"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="210"/>
       <c r="G9" s="73" t="s">
         <v>64</v>
       </c>
@@ -5426,24 +5430,24 @@
       <c r="L9" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="M9" s="212"/>
+      <c r="M9" s="210"/>
     </row>
     <row r="10" spans="1:13" s="58" customFormat="1" ht="18">
-      <c r="A10" s="209" t="s">
+      <c r="A10" s="211" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="210"/>
-      <c r="C10" s="210"/>
-      <c r="D10" s="210"/>
-      <c r="E10" s="210"/>
-      <c r="F10" s="210"/>
-      <c r="G10" s="210"/>
-      <c r="H10" s="210"/>
-      <c r="I10" s="210"/>
-      <c r="J10" s="210"/>
-      <c r="K10" s="210"/>
-      <c r="L10" s="210"/>
-      <c r="M10" s="210"/>
+      <c r="B10" s="212"/>
+      <c r="C10" s="212"/>
+      <c r="D10" s="212"/>
+      <c r="E10" s="212"/>
+      <c r="F10" s="212"/>
+      <c r="G10" s="212"/>
+      <c r="H10" s="212"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="212"/>
+      <c r="K10" s="212"/>
+      <c r="L10" s="212"/>
+      <c r="M10" s="212"/>
     </row>
     <row r="11" spans="1:13" s="58" customFormat="1" ht="33.6">
       <c r="A11" s="75" t="s">
@@ -5570,21 +5574,21 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" s="58" customFormat="1" ht="18">
-      <c r="A15" s="211" t="s">
+      <c r="A15" s="213" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="211"/>
-      <c r="C15" s="211"/>
-      <c r="D15" s="211"/>
-      <c r="E15" s="211"/>
-      <c r="F15" s="211"/>
-      <c r="G15" s="211"/>
-      <c r="H15" s="211"/>
-      <c r="I15" s="211"/>
-      <c r="J15" s="211"/>
-      <c r="K15" s="211"/>
-      <c r="L15" s="211"/>
-      <c r="M15" s="211"/>
+      <c r="B15" s="213"/>
+      <c r="C15" s="213"/>
+      <c r="D15" s="213"/>
+      <c r="E15" s="213"/>
+      <c r="F15" s="213"/>
+      <c r="G15" s="213"/>
+      <c r="H15" s="213"/>
+      <c r="I15" s="213"/>
+      <c r="J15" s="213"/>
+      <c r="K15" s="213"/>
+      <c r="L15" s="213"/>
+      <c r="M15" s="213"/>
     </row>
     <row r="16" spans="1:13" s="58" customFormat="1" ht="67.2">
       <c r="A16" s="15" t="s">
@@ -5798,12 +5802,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
     <mergeCell ref="A10:M10"/>
     <mergeCell ref="A15:M15"/>
     <mergeCell ref="A7:A9"/>
@@ -5813,6 +5811,12 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="M7:M9"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G11:G14 G16:G20 J11:J14 J16:J20" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -5856,25 +5860,25 @@
       <c r="A1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="223" t="s">
+      <c r="B1" s="215" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
     </row>
     <row r="2" spans="1:6" ht="16.8">
       <c r="A2" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="216" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
     </row>
     <row r="3" spans="1:6" ht="16.8">
       <c r="A3" s="38"/>
@@ -5942,64 +5946,64 @@
     <row r="37" spans="1:135" ht="40.200000000000003" customHeight="1"/>
     <row r="38" spans="1:135" ht="40.200000000000003" customHeight="1"/>
     <row r="39" spans="1:135" ht="40.200000000000003" customHeight="1">
-      <c r="A39" s="219" t="s">
+      <c r="A39" s="221" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="219" t="s">
+      <c r="B39" s="221" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="219" t="s">
+      <c r="C39" s="221" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="219" t="s">
+      <c r="D39" s="221" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="222" t="s">
+      <c r="E39" s="224" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="219" t="s">
+      <c r="F39" s="221" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="225" t="s">
+      <c r="G39" s="217" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="217"/>
-      <c r="I39" s="218"/>
-      <c r="J39" s="225" t="s">
+      <c r="H39" s="218"/>
+      <c r="I39" s="219"/>
+      <c r="J39" s="217" t="s">
         <v>62</v>
       </c>
-      <c r="K39" s="217"/>
-      <c r="L39" s="218"/>
-      <c r="M39" s="219" t="s">
+      <c r="K39" s="218"/>
+      <c r="L39" s="219"/>
+      <c r="M39" s="221" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:135" ht="40.200000000000003" customHeight="1">
-      <c r="A40" s="220"/>
-      <c r="B40" s="220"/>
-      <c r="C40" s="220"/>
-      <c r="D40" s="220"/>
-      <c r="E40" s="220"/>
-      <c r="F40" s="220"/>
-      <c r="G40" s="225" t="s">
+      <c r="A40" s="222"/>
+      <c r="B40" s="222"/>
+      <c r="C40" s="222"/>
+      <c r="D40" s="222"/>
+      <c r="E40" s="222"/>
+      <c r="F40" s="222"/>
+      <c r="G40" s="217" t="s">
         <v>19</v>
       </c>
-      <c r="H40" s="217"/>
-      <c r="I40" s="218"/>
-      <c r="J40" s="225" t="s">
+      <c r="H40" s="218"/>
+      <c r="I40" s="219"/>
+      <c r="J40" s="217" t="s">
         <v>20</v>
       </c>
-      <c r="K40" s="217"/>
-      <c r="L40" s="218"/>
-      <c r="M40" s="220"/>
+      <c r="K40" s="218"/>
+      <c r="L40" s="219"/>
+      <c r="M40" s="222"/>
     </row>
     <row r="41" spans="1:135" ht="40.200000000000003" customHeight="1">
-      <c r="A41" s="221"/>
-      <c r="B41" s="221"/>
-      <c r="C41" s="221"/>
-      <c r="D41" s="221"/>
-      <c r="E41" s="221"/>
-      <c r="F41" s="221"/>
+      <c r="A41" s="223"/>
+      <c r="B41" s="223"/>
+      <c r="C41" s="223"/>
+      <c r="D41" s="223"/>
+      <c r="E41" s="223"/>
+      <c r="F41" s="223"/>
       <c r="G41" s="41" t="s">
         <v>64</v>
       </c>
@@ -6018,24 +6022,24 @@
       <c r="L41" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="M41" s="221"/>
+      <c r="M41" s="223"/>
     </row>
     <row r="42" spans="1:135" ht="40.200000000000003" customHeight="1">
-      <c r="A42" s="216" t="s">
+      <c r="A42" s="220" t="s">
         <v>295</v>
       </c>
-      <c r="B42" s="217"/>
-      <c r="C42" s="217"/>
-      <c r="D42" s="217"/>
-      <c r="E42" s="217"/>
-      <c r="F42" s="217"/>
-      <c r="G42" s="217"/>
-      <c r="H42" s="217"/>
-      <c r="I42" s="217"/>
-      <c r="J42" s="217"/>
-      <c r="K42" s="217"/>
-      <c r="L42" s="217"/>
-      <c r="M42" s="218"/>
+      <c r="B42" s="218"/>
+      <c r="C42" s="218"/>
+      <c r="D42" s="218"/>
+      <c r="E42" s="218"/>
+      <c r="F42" s="218"/>
+      <c r="G42" s="218"/>
+      <c r="H42" s="218"/>
+      <c r="I42" s="218"/>
+      <c r="J42" s="218"/>
+      <c r="K42" s="218"/>
+      <c r="L42" s="218"/>
+      <c r="M42" s="219"/>
     </row>
     <row r="43" spans="1:135" s="11" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A43" s="43" t="s">
@@ -7692,12 +7696,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="J40:L40"/>
     <mergeCell ref="A42:M42"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="B39:B41"/>
@@ -7706,6 +7704,12 @@
     <mergeCell ref="E39:E41"/>
     <mergeCell ref="F39:F41"/>
     <mergeCell ref="M39:M41"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="J40:L40"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G43:G50 G52:G55 J43:J50 J52:J55" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -7748,26 +7752,26 @@
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="208" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="22.8">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="239" t="s">
+      <c r="B2" s="225" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="240"/>
-      <c r="D2" s="240"/>
-      <c r="E2" s="240"/>
-      <c r="F2" s="240"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.8">
@@ -7831,62 +7835,62 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="16.8">
-      <c r="A33" s="232" t="s">
+      <c r="A33" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="235" t="s">
+      <c r="B33" s="237" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="235" t="s">
+      <c r="C33" s="237" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="235" t="s">
+      <c r="D33" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="236" t="s">
+      <c r="E33" s="238" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="235" t="s">
+      <c r="F33" s="237" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="237" t="s">
+      <c r="G33" s="227" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="237"/>
-      <c r="I33" s="237"/>
-      <c r="J33" s="237"/>
-      <c r="K33" s="237"/>
-      <c r="L33" s="237"/>
-      <c r="M33" s="237" t="s">
+      <c r="H33" s="227"/>
+      <c r="I33" s="227"/>
+      <c r="J33" s="227"/>
+      <c r="K33" s="227"/>
+      <c r="L33" s="227"/>
+      <c r="M33" s="227" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="16.8">
-      <c r="A34" s="233"/>
-      <c r="B34" s="235"/>
-      <c r="C34" s="235"/>
-      <c r="D34" s="235"/>
-      <c r="E34" s="236"/>
-      <c r="F34" s="235"/>
-      <c r="G34" s="237" t="s">
+      <c r="A34" s="235"/>
+      <c r="B34" s="237"/>
+      <c r="C34" s="237"/>
+      <c r="D34" s="237"/>
+      <c r="E34" s="238"/>
+      <c r="F34" s="237"/>
+      <c r="G34" s="227" t="s">
         <v>19</v>
       </c>
-      <c r="H34" s="237"/>
-      <c r="I34" s="237"/>
-      <c r="J34" s="237" t="s">
+      <c r="H34" s="227"/>
+      <c r="I34" s="227"/>
+      <c r="J34" s="227" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="237"/>
-      <c r="L34" s="237"/>
-      <c r="M34" s="238"/>
+      <c r="K34" s="227"/>
+      <c r="L34" s="227"/>
+      <c r="M34" s="239"/>
     </row>
     <row r="35" spans="1:13" ht="16.8">
-      <c r="A35" s="234"/>
-      <c r="B35" s="235"/>
-      <c r="C35" s="235"/>
-      <c r="D35" s="235"/>
-      <c r="E35" s="236"/>
-      <c r="F35" s="235"/>
+      <c r="A35" s="236"/>
+      <c r="B35" s="237"/>
+      <c r="C35" s="237"/>
+      <c r="D35" s="237"/>
+      <c r="E35" s="238"/>
+      <c r="F35" s="237"/>
       <c r="G35" s="9" t="s">
         <v>64</v>
       </c>
@@ -7905,24 +7909,24 @@
       <c r="L35" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="M35" s="238"/>
+      <c r="M35" s="239"/>
     </row>
     <row r="36" spans="1:13" ht="16.8">
-      <c r="A36" s="226" t="s">
+      <c r="A36" s="228" t="s">
         <v>298</v>
       </c>
-      <c r="B36" s="227"/>
-      <c r="C36" s="227"/>
-      <c r="D36" s="227"/>
-      <c r="E36" s="227"/>
-      <c r="F36" s="227"/>
-      <c r="G36" s="227"/>
-      <c r="H36" s="227"/>
-      <c r="I36" s="227"/>
-      <c r="J36" s="227"/>
-      <c r="K36" s="227"/>
-      <c r="L36" s="227"/>
-      <c r="M36" s="228"/>
+      <c r="B36" s="229"/>
+      <c r="C36" s="229"/>
+      <c r="D36" s="229"/>
+      <c r="E36" s="229"/>
+      <c r="F36" s="229"/>
+      <c r="G36" s="229"/>
+      <c r="H36" s="229"/>
+      <c r="I36" s="229"/>
+      <c r="J36" s="229"/>
+      <c r="K36" s="229"/>
+      <c r="L36" s="229"/>
+      <c r="M36" s="230"/>
     </row>
     <row r="37" spans="1:13" ht="40.200000000000003" customHeight="1">
       <c r="A37" s="11" t="s">
@@ -7991,21 +7995,21 @@
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="40.200000000000003" customHeight="1">
-      <c r="A39" s="229" t="s">
+      <c r="A39" s="231" t="s">
         <v>299</v>
       </c>
-      <c r="B39" s="230"/>
-      <c r="C39" s="230"/>
-      <c r="D39" s="230"/>
-      <c r="E39" s="230"/>
-      <c r="F39" s="230"/>
-      <c r="G39" s="230"/>
-      <c r="H39" s="230"/>
-      <c r="I39" s="230"/>
-      <c r="J39" s="230"/>
-      <c r="K39" s="230"/>
-      <c r="L39" s="230"/>
-      <c r="M39" s="231"/>
+      <c r="B39" s="232"/>
+      <c r="C39" s="232"/>
+      <c r="D39" s="232"/>
+      <c r="E39" s="232"/>
+      <c r="F39" s="232"/>
+      <c r="G39" s="232"/>
+      <c r="H39" s="232"/>
+      <c r="I39" s="232"/>
+      <c r="J39" s="232"/>
+      <c r="K39" s="232"/>
+      <c r="L39" s="232"/>
+      <c r="M39" s="233"/>
     </row>
     <row r="40" spans="1:13" ht="91.05" customHeight="1">
       <c r="A40" s="14" t="s">
@@ -8178,11 +8182,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G33:L33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:L34"/>
     <mergeCell ref="A36:M36"/>
     <mergeCell ref="A39:M39"/>
     <mergeCell ref="A33:A35"/>
@@ -8192,6 +8191,11 @@
     <mergeCell ref="E33:E35"/>
     <mergeCell ref="F33:F35"/>
     <mergeCell ref="M33:M35"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G33:L33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:L34"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G37:G38 G40:G46 J37:J38 J40:J46" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -8234,26 +8238,26 @@
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="208" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="22.8">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="240" t="s">
+      <c r="B2" s="226" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="240"/>
-      <c r="D2" s="240"/>
-      <c r="E2" s="240"/>
-      <c r="F2" s="240"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.8">
@@ -8320,62 +8324,62 @@
       <c r="J18" s="35"/>
     </row>
     <row r="31" spans="1:13" ht="16.8">
-      <c r="A31" s="232" t="s">
+      <c r="A31" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="235" t="s">
+      <c r="B31" s="237" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="235" t="s">
+      <c r="C31" s="237" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="235" t="s">
+      <c r="D31" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="236" t="s">
+      <c r="E31" s="238" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="235" t="s">
+      <c r="F31" s="237" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="237" t="s">
+      <c r="G31" s="227" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="237"/>
-      <c r="I31" s="237"/>
-      <c r="J31" s="237"/>
-      <c r="K31" s="237"/>
-      <c r="L31" s="237"/>
-      <c r="M31" s="237" t="s">
+      <c r="H31" s="227"/>
+      <c r="I31" s="227"/>
+      <c r="J31" s="227"/>
+      <c r="K31" s="227"/>
+      <c r="L31" s="227"/>
+      <c r="M31" s="227" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="16.8">
-      <c r="A32" s="233"/>
-      <c r="B32" s="235"/>
-      <c r="C32" s="235"/>
-      <c r="D32" s="235"/>
-      <c r="E32" s="236"/>
-      <c r="F32" s="235"/>
-      <c r="G32" s="237" t="s">
+      <c r="A32" s="235"/>
+      <c r="B32" s="237"/>
+      <c r="C32" s="237"/>
+      <c r="D32" s="237"/>
+      <c r="E32" s="238"/>
+      <c r="F32" s="237"/>
+      <c r="G32" s="227" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="237"/>
-      <c r="I32" s="237"/>
-      <c r="J32" s="237" t="s">
+      <c r="H32" s="227"/>
+      <c r="I32" s="227"/>
+      <c r="J32" s="227" t="s">
         <v>20</v>
       </c>
-      <c r="K32" s="237"/>
-      <c r="L32" s="237"/>
-      <c r="M32" s="238"/>
+      <c r="K32" s="227"/>
+      <c r="L32" s="227"/>
+      <c r="M32" s="239"/>
     </row>
     <row r="33" spans="1:13" ht="16.8">
-      <c r="A33" s="234"/>
-      <c r="B33" s="235"/>
-      <c r="C33" s="235"/>
-      <c r="D33" s="235"/>
-      <c r="E33" s="236"/>
-      <c r="F33" s="235"/>
+      <c r="A33" s="236"/>
+      <c r="B33" s="237"/>
+      <c r="C33" s="237"/>
+      <c r="D33" s="237"/>
+      <c r="E33" s="238"/>
+      <c r="F33" s="237"/>
       <c r="G33" s="9" t="s">
         <v>64</v>
       </c>
@@ -8394,24 +8398,24 @@
       <c r="L33" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="M33" s="238"/>
+      <c r="M33" s="239"/>
     </row>
     <row r="34" spans="1:13" ht="16.8">
-      <c r="A34" s="241" t="s">
+      <c r="A34" s="240" t="s">
         <v>213</v>
       </c>
-      <c r="B34" s="227"/>
-      <c r="C34" s="227"/>
-      <c r="D34" s="227"/>
-      <c r="E34" s="227"/>
-      <c r="F34" s="227"/>
-      <c r="G34" s="227"/>
-      <c r="H34" s="227"/>
-      <c r="I34" s="227"/>
-      <c r="J34" s="227"/>
-      <c r="K34" s="227"/>
-      <c r="L34" s="227"/>
-      <c r="M34" s="228"/>
+      <c r="B34" s="229"/>
+      <c r="C34" s="229"/>
+      <c r="D34" s="229"/>
+      <c r="E34" s="229"/>
+      <c r="F34" s="229"/>
+      <c r="G34" s="229"/>
+      <c r="H34" s="229"/>
+      <c r="I34" s="229"/>
+      <c r="J34" s="229"/>
+      <c r="K34" s="229"/>
+      <c r="L34" s="229"/>
+      <c r="M34" s="230"/>
     </row>
     <row r="35" spans="1:13" ht="40.200000000000003" customHeight="1">
       <c r="A35" s="11" t="s">
@@ -8579,21 +8583,21 @@
       <c r="M39" s="3"/>
     </row>
     <row r="40" spans="1:13" ht="40.200000000000003" customHeight="1">
-      <c r="A40" s="242" t="s">
+      <c r="A40" s="241" t="s">
         <v>196</v>
       </c>
-      <c r="B40" s="230"/>
-      <c r="C40" s="230"/>
-      <c r="D40" s="230"/>
-      <c r="E40" s="230"/>
-      <c r="F40" s="230"/>
-      <c r="G40" s="230"/>
-      <c r="H40" s="230"/>
-      <c r="I40" s="230"/>
-      <c r="J40" s="230"/>
-      <c r="K40" s="230"/>
-      <c r="L40" s="230"/>
-      <c r="M40" s="231"/>
+      <c r="B40" s="232"/>
+      <c r="C40" s="232"/>
+      <c r="D40" s="232"/>
+      <c r="E40" s="232"/>
+      <c r="F40" s="232"/>
+      <c r="G40" s="232"/>
+      <c r="H40" s="232"/>
+      <c r="I40" s="232"/>
+      <c r="J40" s="232"/>
+      <c r="K40" s="232"/>
+      <c r="L40" s="232"/>
+      <c r="M40" s="233"/>
     </row>
     <row r="41" spans="1:13" ht="119.4" customHeight="1">
       <c r="A41" s="14" t="s">
@@ -8690,11 +8694,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G31:L31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
     <mergeCell ref="A34:M34"/>
     <mergeCell ref="A40:M40"/>
     <mergeCell ref="A31:A33"/>
@@ -8704,6 +8703,11 @@
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="F31:F33"/>
     <mergeCell ref="M31:M33"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G31:L31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G35:G39 G41:G47 J35:J39 J41:J47" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -8758,13 +8762,13 @@
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="240" t="s">
+      <c r="B2" s="226" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="240"/>
-      <c r="D2" s="240"/>
-      <c r="E2" s="240"/>
-      <c r="F2" s="240"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.8">
@@ -8828,62 +8832,62 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="17.399999999999999">
-      <c r="A31" s="246" t="s">
+      <c r="A31" s="249" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="246" t="s">
+      <c r="B31" s="249" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="246" t="s">
+      <c r="C31" s="249" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="246" t="s">
+      <c r="D31" s="249" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="247" t="s">
+      <c r="E31" s="250" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="246" t="s">
+      <c r="F31" s="249" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="250" t="s">
+      <c r="G31" s="242" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="250"/>
-      <c r="I31" s="250"/>
-      <c r="J31" s="250"/>
-      <c r="K31" s="250"/>
-      <c r="L31" s="250"/>
-      <c r="M31" s="248" t="s">
+      <c r="H31" s="242"/>
+      <c r="I31" s="242"/>
+      <c r="J31" s="242"/>
+      <c r="K31" s="242"/>
+      <c r="L31" s="242"/>
+      <c r="M31" s="251" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="17.399999999999999">
-      <c r="A32" s="246"/>
-      <c r="B32" s="246"/>
-      <c r="C32" s="246"/>
-      <c r="D32" s="246"/>
-      <c r="E32" s="247"/>
-      <c r="F32" s="246"/>
-      <c r="G32" s="250" t="s">
+      <c r="A32" s="249"/>
+      <c r="B32" s="249"/>
+      <c r="C32" s="249"/>
+      <c r="D32" s="249"/>
+      <c r="E32" s="250"/>
+      <c r="F32" s="249"/>
+      <c r="G32" s="242" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="250"/>
-      <c r="I32" s="250"/>
-      <c r="J32" s="250" t="s">
+      <c r="H32" s="242"/>
+      <c r="I32" s="242"/>
+      <c r="J32" s="242" t="s">
         <v>20</v>
       </c>
-      <c r="K32" s="250"/>
-      <c r="L32" s="250"/>
-      <c r="M32" s="249"/>
+      <c r="K32" s="242"/>
+      <c r="L32" s="242"/>
+      <c r="M32" s="252"/>
     </row>
     <row r="33" spans="1:13" ht="15.6">
-      <c r="A33" s="246"/>
-      <c r="B33" s="246"/>
-      <c r="C33" s="246"/>
-      <c r="D33" s="246"/>
-      <c r="E33" s="247"/>
-      <c r="F33" s="246"/>
+      <c r="A33" s="249"/>
+      <c r="B33" s="249"/>
+      <c r="C33" s="249"/>
+      <c r="D33" s="249"/>
+      <c r="E33" s="250"/>
+      <c r="F33" s="249"/>
       <c r="G33" s="22" t="s">
         <v>64</v>
       </c>
@@ -8902,24 +8906,24 @@
       <c r="L33" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="M33" s="249"/>
+      <c r="M33" s="252"/>
     </row>
     <row r="34" spans="1:13" ht="15.6">
-      <c r="A34" s="251" t="s">
+      <c r="A34" s="243" t="s">
         <v>233</v>
       </c>
-      <c r="B34" s="252"/>
-      <c r="C34" s="252"/>
-      <c r="D34" s="252"/>
-      <c r="E34" s="252"/>
-      <c r="F34" s="252"/>
-      <c r="G34" s="252"/>
-      <c r="H34" s="252"/>
-      <c r="I34" s="252"/>
-      <c r="J34" s="252"/>
-      <c r="K34" s="252"/>
-      <c r="L34" s="252"/>
-      <c r="M34" s="253"/>
+      <c r="B34" s="244"/>
+      <c r="C34" s="244"/>
+      <c r="D34" s="244"/>
+      <c r="E34" s="244"/>
+      <c r="F34" s="244"/>
+      <c r="G34" s="244"/>
+      <c r="H34" s="244"/>
+      <c r="I34" s="244"/>
+      <c r="J34" s="244"/>
+      <c r="K34" s="244"/>
+      <c r="L34" s="244"/>
+      <c r="M34" s="245"/>
     </row>
     <row r="35" spans="1:13" ht="33.6">
       <c r="A35" s="24" t="s">
@@ -9000,21 +9004,21 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="16.8">
-      <c r="A37" s="243" t="s">
+      <c r="A37" s="246" t="s">
         <v>241</v>
       </c>
-      <c r="B37" s="244"/>
-      <c r="C37" s="244"/>
-      <c r="D37" s="244"/>
-      <c r="E37" s="244"/>
-      <c r="F37" s="244"/>
-      <c r="G37" s="244"/>
-      <c r="H37" s="244"/>
-      <c r="I37" s="244"/>
-      <c r="J37" s="244"/>
-      <c r="K37" s="244"/>
-      <c r="L37" s="244"/>
-      <c r="M37" s="245"/>
+      <c r="B37" s="247"/>
+      <c r="C37" s="247"/>
+      <c r="D37" s="247"/>
+      <c r="E37" s="247"/>
+      <c r="F37" s="247"/>
+      <c r="G37" s="247"/>
+      <c r="H37" s="247"/>
+      <c r="I37" s="247"/>
+      <c r="J37" s="247"/>
+      <c r="K37" s="247"/>
+      <c r="L37" s="247"/>
+      <c r="M37" s="248"/>
     </row>
     <row r="38" spans="1:13" ht="134.4">
       <c r="A38" s="15" t="s">
@@ -9486,11 +9490,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G31:L31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="A34:M34"/>
     <mergeCell ref="A37:M37"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="B31:B33"/>
@@ -9499,6 +9498,11 @@
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="F31:F33"/>
     <mergeCell ref="M31:M33"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G31:L31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="A34:M34"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G35:G36 G38:G49 J35:J36" xr:uid="{00000000-0002-0000-0700-000000000000}">
@@ -9517,7 +9521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
@@ -9541,26 +9545,26 @@
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="214" t="s">
+      <c r="B1" s="208" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="22.8">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="240" t="s">
+      <c r="B2" s="226" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="240"/>
-      <c r="D2" s="240"/>
-      <c r="E2" s="240"/>
-      <c r="F2" s="240"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.8">
@@ -9624,62 +9628,62 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="16.8">
-      <c r="A26" s="232" t="s">
+      <c r="A26" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="235" t="s">
+      <c r="B26" s="237" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="235" t="s">
+      <c r="C26" s="237" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="235" t="s">
+      <c r="D26" s="237" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="236" t="s">
+      <c r="E26" s="238" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="235" t="s">
+      <c r="F26" s="237" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="237" t="s">
+      <c r="G26" s="227" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="237"/>
-      <c r="I26" s="237"/>
-      <c r="J26" s="237"/>
-      <c r="K26" s="237"/>
-      <c r="L26" s="237"/>
-      <c r="M26" s="237" t="s">
+      <c r="H26" s="227"/>
+      <c r="I26" s="227"/>
+      <c r="J26" s="227"/>
+      <c r="K26" s="227"/>
+      <c r="L26" s="227"/>
+      <c r="M26" s="227" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="16.8">
-      <c r="A27" s="233"/>
-      <c r="B27" s="235"/>
-      <c r="C27" s="235"/>
-      <c r="D27" s="235"/>
-      <c r="E27" s="236"/>
-      <c r="F27" s="235"/>
-      <c r="G27" s="237" t="s">
+      <c r="A27" s="235"/>
+      <c r="B27" s="237"/>
+      <c r="C27" s="237"/>
+      <c r="D27" s="237"/>
+      <c r="E27" s="238"/>
+      <c r="F27" s="237"/>
+      <c r="G27" s="227" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="237"/>
-      <c r="I27" s="237"/>
-      <c r="J27" s="237" t="s">
+      <c r="H27" s="227"/>
+      <c r="I27" s="227"/>
+      <c r="J27" s="227" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="237"/>
-      <c r="L27" s="237"/>
-      <c r="M27" s="238"/>
+      <c r="K27" s="227"/>
+      <c r="L27" s="227"/>
+      <c r="M27" s="239"/>
     </row>
     <row r="28" spans="1:13" ht="16.8">
-      <c r="A28" s="234"/>
-      <c r="B28" s="235"/>
-      <c r="C28" s="235"/>
-      <c r="D28" s="235"/>
-      <c r="E28" s="236"/>
-      <c r="F28" s="235"/>
+      <c r="A28" s="236"/>
+      <c r="B28" s="237"/>
+      <c r="C28" s="237"/>
+      <c r="D28" s="237"/>
+      <c r="E28" s="238"/>
+      <c r="F28" s="237"/>
       <c r="G28" s="9" t="s">
         <v>64</v>
       </c>
@@ -9698,24 +9702,24 @@
       <c r="L28" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="M28" s="238"/>
+      <c r="M28" s="239"/>
     </row>
     <row r="29" spans="1:13" ht="16.8">
-      <c r="A29" s="241" t="s">
+      <c r="A29" s="240" t="s">
         <v>190</v>
       </c>
-      <c r="B29" s="227"/>
-      <c r="C29" s="227"/>
-      <c r="D29" s="227"/>
-      <c r="E29" s="227"/>
-      <c r="F29" s="227"/>
-      <c r="G29" s="227"/>
-      <c r="H29" s="227"/>
-      <c r="I29" s="227"/>
-      <c r="J29" s="227"/>
-      <c r="K29" s="227"/>
-      <c r="L29" s="227"/>
-      <c r="M29" s="228"/>
+      <c r="B29" s="229"/>
+      <c r="C29" s="229"/>
+      <c r="D29" s="229"/>
+      <c r="E29" s="229"/>
+      <c r="F29" s="229"/>
+      <c r="G29" s="229"/>
+      <c r="H29" s="229"/>
+      <c r="I29" s="229"/>
+      <c r="J29" s="229"/>
+      <c r="K29" s="229"/>
+      <c r="L29" s="229"/>
+      <c r="M29" s="230"/>
     </row>
     <row r="30" spans="1:13" ht="40.200000000000003" customHeight="1">
       <c r="A30" s="11" t="s">
@@ -9850,21 +9854,21 @@
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" ht="40.200000000000003" customHeight="1">
-      <c r="A34" s="229" t="s">
+      <c r="A34" s="231" t="s">
         <v>297</v>
       </c>
-      <c r="B34" s="230"/>
-      <c r="C34" s="230"/>
-      <c r="D34" s="230"/>
-      <c r="E34" s="230"/>
-      <c r="F34" s="230"/>
-      <c r="G34" s="230"/>
-      <c r="H34" s="230"/>
-      <c r="I34" s="230"/>
-      <c r="J34" s="230"/>
-      <c r="K34" s="230"/>
-      <c r="L34" s="230"/>
-      <c r="M34" s="231"/>
+      <c r="B34" s="232"/>
+      <c r="C34" s="232"/>
+      <c r="D34" s="232"/>
+      <c r="E34" s="232"/>
+      <c r="F34" s="232"/>
+      <c r="G34" s="232"/>
+      <c r="H34" s="232"/>
+      <c r="I34" s="232"/>
+      <c r="J34" s="232"/>
+      <c r="K34" s="232"/>
+      <c r="L34" s="232"/>
+      <c r="M34" s="233"/>
     </row>
     <row r="35" spans="1:13" ht="91.05" customHeight="1">
       <c r="A35" s="14" t="s">
@@ -9959,11 +9963,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:L27"/>
     <mergeCell ref="A29:M29"/>
     <mergeCell ref="A34:M34"/>
     <mergeCell ref="A26:A28"/>
@@ -9973,6 +9972,11 @@
     <mergeCell ref="E26:E28"/>
     <mergeCell ref="F26:F28"/>
     <mergeCell ref="M26:M28"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:L27"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G30:G33 G35:G41 J30:J33 J35:J41" xr:uid="{00000000-0002-0000-0800-000000000000}">

</xml_diff>